<commit_message>
Add new entries to CSV and PDF files; refactor file paths in Excel and Word functions for improved directory handling
</commit_message>
<xml_diff>
--- a/Temp/temp2.xlsx
+++ b/Temp/temp2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Fiverr Projects\Latest New\4-   450usd\Project-Acceptance_PyQT5\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Study\Fiverr Projects\Latest New\4-   450usd\Project-Acceptance_PyQT5\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69FDE43E-1BA9-46AF-AEDD-F599FDDCEC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3546650-AC8E-4644-8B6D-EEF145352912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Infrastructure Type</t>
   </si>
@@ -58,16 +58,25 @@
     <t>asdsa</t>
   </si>
   <si>
+    <t>new</t>
+  </si>
+  <si>
     <t>dsa</t>
   </si>
   <si>
     <t>asd</t>
   </si>
   <si>
+    <t>king</t>
+  </si>
+  <si>
     <t>dsaf</t>
   </si>
   <si>
     <t>ads</t>
+  </si>
+  <si>
+    <t>das</t>
   </si>
   <si>
     <t>Accepted</t>
@@ -481,7 +490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,16 +527,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -544,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -558,16 +567,36 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +611,7 @@
       <formula>NOT(ISERROR(SEARCH("Removed",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I4">
+  <conditionalFormatting sqref="B2:I5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="4">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>